<commit_message>
fixed scraping and analysis
</commit_message>
<xml_diff>
--- a/data_analysis/replies_averages.xlsx
+++ b/data_analysis/replies_averages.xlsx
@@ -3063,7 +3063,7 @@
         <v>32</v>
       </c>
       <c r="E33">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F33">
         <v>2</v>
@@ -3589,7 +3589,7 @@
         <v>32</v>
       </c>
       <c r="E18">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F18">
         <v>2</v>
@@ -4115,7 +4115,7 @@
         <v>32</v>
       </c>
       <c r="E18">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F18">
         <v>5</v>
@@ -5453,7 +5453,7 @@
         <v>32</v>
       </c>
       <c r="E46">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F46">
         <v>1</v>
@@ -6414,7 +6414,7 @@
         <v>32</v>
       </c>
       <c r="E33">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F33">
         <v>5</v>
@@ -7694,7 +7694,7 @@
         <v>32</v>
       </c>
       <c r="E44">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="F44">
         <v>23</v>
@@ -10888,7 +10888,7 @@
         <v>32</v>
       </c>
       <c r="E110">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="F110">
         <v>92</v>

</xml_diff>